<commit_message>
Fix hydrogen BTU conversion
</commit_message>
<xml_diff>
--- a/InputData/web-app/BCF/BTU Conversion Factors.xlsx
+++ b/InputData/web-app/BCF/BTU Conversion Factors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-brazil\InputData\web-app\BCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-brazil\InputData\web-app\BCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
   <definedNames>
     <definedName name="gal_per_barrel">About!$A$63</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -15642,8 +15642,8 @@
   </sheetPr>
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="AA34" sqref="AA34"/>
+    <sheetView topLeftCell="X13" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:AI22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -18449,140 +18449,140 @@
         <v>368</v>
       </c>
       <c r="B22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="C22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="D22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="E22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="F22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="G22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="H22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="I22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="J22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="K22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="L22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="M22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="N22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="O22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="P22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="Q22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="R22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="S22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="T22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="U22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="V22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="W22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="X22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="Y22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="Z22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AA22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AB22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AC22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AD22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AE22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AF22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AG22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AH22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AI22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^9*About!$D$50</f>
+        <v>134509803921.56865</v>
       </c>
     </row>
   </sheetData>
@@ -18597,8 +18597,8 @@
   </sheetPr>
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="U10" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:AI22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -21404,140 +21404,140 @@
         <v>368</v>
       </c>
       <c r="B22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="C22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="D22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="E22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="F22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="G22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="H22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="I22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="J22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="K22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="L22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="M22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="N22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="O22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="P22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="Q22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="R22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="S22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="T22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="U22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="V22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="W22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="X22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="Y22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="Z22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AA22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AB22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AC22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AD22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AE22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AF22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AG22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AH22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AI22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$61*'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$61/'GREET1 Fuel_Specs'!$E$61*10^3*About!$D$41</f>
+        <v>134509.80392156864</v>
       </c>
     </row>
   </sheetData>

</xml_diff>